<commit_message>
Archivos de planeación anual
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Métricas y monitoreo/Plan_Métricas_2016.xlsx
+++ b/Proyectos/2016/Métricas y monitoreo/Plan_Métricas_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Objetivos de Medición" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,6 +19,11 @@
     <sheet name="Índice de Satisfacción" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -179,6 +184,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Guía de análisis:</t>
     </r>
     <r>
@@ -385,6 +396,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t>Guía de análisis:</t>
     </r>
     <r>
@@ -656,10 +673,10 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -1006,12 +1023,13 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1034,6 +1052,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1041,6 +1060,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1136,6 +1156,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1143,6 +1164,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1238,6 +1260,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1245,6 +1268,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1320,16 +1344,17 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="51254902"/>
-        <c:axId val="94988994"/>
+        <c:axId val="72435166"/>
+        <c:axId val="13793230"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51254902"/>
+        <c:axId val="72435166"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1341,14 +1366,32 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="94988994"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="13793230"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94988994"/>
+        <c:axId val="13793230"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,17 +1410,32 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
+                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -1385,8 +1443,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1398,7 +1457,25 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="51254902"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="72435166"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -1416,6 +1493,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1431,12 +1509,13 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1457,6 +1536,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1464,6 +1544,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1557,6 +1638,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1564,6 +1646,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1657,6 +1740,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1664,6 +1748,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1739,16 +1824,17 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="55230506"/>
-        <c:axId val="72537702"/>
+        <c:axId val="18027514"/>
+        <c:axId val="80308284"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="55230506"/>
+        <c:axId val="18027514"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1760,14 +1846,32 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="72537702"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="80308284"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72537702"/>
+        <c:axId val="80308284"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,17 +1890,32 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
+                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -1804,8 +1923,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="\$#,##0.00;[RED]\$#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1817,7 +1937,25 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55230506"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="18027514"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -1835,6 +1973,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1850,12 +1989,13 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1878,6 +2018,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1885,6 +2026,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1980,6 +2122,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1987,6 +2130,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2082,6 +2226,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2089,6 +2234,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2164,16 +2310,17 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="77386939"/>
-        <c:axId val="95363558"/>
+        <c:axId val="98391957"/>
+        <c:axId val="63067750"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77386939"/>
+        <c:axId val="98391957"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2185,14 +2332,32 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="95363558"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="63067750"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95363558"/>
+        <c:axId val="63067750"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2211,17 +2376,32 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
+                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -2229,8 +2409,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2242,7 +2423,25 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="77386939"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="98391957"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -2260,6 +2459,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2275,12 +2475,13 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2303,6 +2504,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2310,6 +2512,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2405,6 +2608,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2412,6 +2616,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2507,6 +2712,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2514,6 +2720,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2589,16 +2796,17 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="79587026"/>
-        <c:axId val="15157086"/>
+        <c:axId val="92254162"/>
+        <c:axId val="70893083"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79587026"/>
+        <c:axId val="92254162"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2610,14 +2818,32 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="15157086"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="70893083"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15157086"/>
+        <c:axId val="70893083"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2636,17 +2862,32 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
+                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -2654,8 +2895,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2667,7 +2909,25 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="79587026"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="92254162"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -2685,6 +2945,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2700,12 +2961,13 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2728,6 +2990,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2735,6 +2998,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2830,6 +3094,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2837,6 +3102,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2932,6 +3198,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2939,6 +3206,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3014,16 +3282,17 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="34436467"/>
-        <c:axId val="54605698"/>
+        <c:axId val="65908345"/>
+        <c:axId val="86565072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="34436467"/>
+        <c:axId val="65908345"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3035,14 +3304,32 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="54605698"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="86565072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54605698"/>
+        <c:axId val="86565072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3061,17 +3348,32 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
+                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -3079,8 +3381,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3092,7 +3395,25 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="34436467"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65908345"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -3110,6 +3431,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3125,12 +3447,13 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
-      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3153,6 +3476,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -3160,6 +3484,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3255,6 +3580,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -3262,6 +3588,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3357,6 +3684,7 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -3364,6 +3692,7 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3439,16 +3768,17 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="83753503"/>
-        <c:axId val="80162291"/>
+        <c:axId val="60765664"/>
+        <c:axId val="95054219"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83753503"/>
+        <c:axId val="60765664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3460,14 +3790,32 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80162291"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95054219"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80162291"/>
+        <c:axId val="95054219"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3486,17 +3834,32 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000">
+                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -3504,8 +3867,9 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3517,7 +3881,25 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="83753503"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60765664"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -3535,6 +3917,7 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3552,15 +3935,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>444600</xdr:colOff>
+      <xdr:colOff>471600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>135720</xdr:rowOff>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>327600</xdr:colOff>
+      <xdr:colOff>354240</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3568,8 +3951,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="44059320" y="9339120"/>
-        <a:ext cx="5979240" cy="2882880"/>
+        <a:off x="34513920" y="9330120"/>
+        <a:ext cx="4626000" cy="2882520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3582,15 +3965,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>216000</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>120960</xdr:rowOff>
+      <xdr:rowOff>111960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3285360</xdr:colOff>
+      <xdr:colOff>3312000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2042280</xdr:rowOff>
+      <xdr:rowOff>2032920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3603,8 +3986,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="419040" y="689760"/>
-          <a:ext cx="5978160" cy="2111760"/>
+          <a:off x="395280" y="680760"/>
+          <a:ext cx="5345280" cy="2111400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3619,15 +4002,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3473640</xdr:colOff>
+      <xdr:colOff>3500640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7452360</xdr:colOff>
+      <xdr:colOff>7479000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1998000</xdr:rowOff>
+      <xdr:rowOff>1988640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3640,8 +4023,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6585480" y="747000"/>
-          <a:ext cx="3978720" cy="2010240"/>
+          <a:off x="5929200" y="738000"/>
+          <a:ext cx="3978360" cy="2009880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3661,15 +4044,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>393840</xdr:colOff>
+      <xdr:colOff>420840</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>41040</xdr:rowOff>
+      <xdr:rowOff>32040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>365400</xdr:colOff>
+      <xdr:colOff>392040</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3677,8 +4060,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="43246080" y="9845280"/>
-        <a:ext cx="8099640" cy="3350160"/>
+        <a:off x="33853320" y="9836280"/>
+        <a:ext cx="6296040" cy="3349800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3691,15 +4074,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>216000</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>308880</xdr:rowOff>
+      <xdr:rowOff>299880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2194200</xdr:colOff>
+      <xdr:colOff>2220840</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2193120</xdr:rowOff>
+      <xdr:rowOff>2183760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3712,8 +4095,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="419040" y="880200"/>
-          <a:ext cx="4887000" cy="2434680"/>
+          <a:off x="395280" y="871200"/>
+          <a:ext cx="4254120" cy="2434320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3728,15 +4111,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2216160</xdr:colOff>
+      <xdr:colOff>2243160</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>280440</xdr:rowOff>
+      <xdr:rowOff>271440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>232200</xdr:colOff>
+      <xdr:colOff>258840</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2181600</xdr:rowOff>
+      <xdr:rowOff>2172240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3749,8 +4132,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5328000" y="851760"/>
-          <a:ext cx="5967720" cy="2451600"/>
+          <a:off x="4671720" y="842760"/>
+          <a:ext cx="4254840" cy="2451240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3770,15 +4153,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>444600</xdr:colOff>
+      <xdr:colOff>471600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:rowOff>60840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>327600</xdr:colOff>
+      <xdr:colOff>354240</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3786,8 +4169,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="45558720" y="9062640"/>
-        <a:ext cx="5978880" cy="2883240"/>
+        <a:off x="35685360" y="9053640"/>
+        <a:ext cx="4626000" cy="2882880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3800,15 +4183,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>216000</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
+      <xdr:rowOff>110880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4064400</xdr:colOff>
+      <xdr:colOff>4091040</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2298240</xdr:rowOff>
+      <xdr:rowOff>2288880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3821,8 +4204,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="419040" y="727920"/>
-          <a:ext cx="6757200" cy="2368800"/>
+          <a:off x="395280" y="718920"/>
+          <a:ext cx="6124320" cy="2368440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3837,15 +4220,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4730760</xdr:colOff>
+      <xdr:colOff>4757760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>34200</xdr:rowOff>
+      <xdr:rowOff>25200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>8528400</xdr:colOff>
+      <xdr:colOff>8555040</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2275920</xdr:rowOff>
+      <xdr:rowOff>2266560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3858,8 +4241,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7842600" y="642240"/>
-          <a:ext cx="3797640" cy="2432160"/>
+          <a:off x="7186320" y="633240"/>
+          <a:ext cx="3797280" cy="2431800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3879,15 +4262,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>444600</xdr:colOff>
+      <xdr:colOff>471600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>68760</xdr:rowOff>
+      <xdr:rowOff>59760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>327600</xdr:colOff>
+      <xdr:colOff>354240</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>94320</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3895,8 +4278,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="42598800" y="9281880"/>
-        <a:ext cx="5979240" cy="2882880"/>
+        <a:off x="33361200" y="9272880"/>
+        <a:ext cx="4626000" cy="2882520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3909,15 +4292,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>216000</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>118440</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2220840</xdr:colOff>
+      <xdr:colOff>2247480</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2334960</xdr:rowOff>
+      <xdr:rowOff>2325600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3930,8 +4313,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="419040" y="880200"/>
-          <a:ext cx="4913640" cy="2406960"/>
+          <a:off x="395280" y="871200"/>
+          <a:ext cx="4280760" cy="2406600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3946,15 +4329,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2247120</xdr:colOff>
+      <xdr:colOff>2274120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>99360</xdr:rowOff>
+      <xdr:rowOff>90360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6394680</xdr:colOff>
+      <xdr:colOff>6421320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2349720</xdr:rowOff>
+      <xdr:rowOff>2340360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3967,8 +4350,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5358960" y="861120"/>
-          <a:ext cx="4147560" cy="2440800"/>
+          <a:off x="4702680" y="852120"/>
+          <a:ext cx="4147200" cy="2440440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3988,15 +4371,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>444600</xdr:colOff>
+      <xdr:colOff>471600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>68760</xdr:rowOff>
+      <xdr:rowOff>59760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>327600</xdr:colOff>
+      <xdr:colOff>354240</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>94320</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4004,8 +4387,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="42116400" y="9203760"/>
-        <a:ext cx="5978880" cy="2882880"/>
+        <a:off x="32980320" y="9194760"/>
+        <a:ext cx="4626000" cy="2882520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4018,15 +4401,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1006560</xdr:colOff>
+      <xdr:colOff>1033560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>118440</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2613240</xdr:colOff>
+      <xdr:colOff>2639880</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2355840</xdr:rowOff>
+      <xdr:rowOff>2346480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4039,8 +4422,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1209600" y="689760"/>
-          <a:ext cx="4515480" cy="2427840"/>
+          <a:off x="1185840" y="680760"/>
+          <a:ext cx="3882600" cy="2427480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4060,15 +4443,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>444600</xdr:colOff>
+      <xdr:colOff>471600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>327600</xdr:colOff>
+      <xdr:colOff>354240</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>95400</xdr:rowOff>
+      <xdr:rowOff>86040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4076,8 +4459,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="42395760" y="9118080"/>
-        <a:ext cx="5978880" cy="2882880"/>
+        <a:off x="33199200" y="9109080"/>
+        <a:ext cx="4626360" cy="2882520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4090,15 +4473,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>663840</xdr:colOff>
+      <xdr:colOff>690840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>146880</xdr:rowOff>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2089800</xdr:colOff>
+      <xdr:colOff>2116440</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2271600</xdr:rowOff>
+      <xdr:rowOff>2262240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4111,8 +4494,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="866880" y="718200"/>
-          <a:ext cx="4334760" cy="2315160"/>
+          <a:off x="843120" y="709200"/>
+          <a:ext cx="3701880" cy="2314800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4132,15 +4515,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1034640</xdr:colOff>
+      <xdr:colOff>1061640</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>32760</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4327560</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>277560</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1697040</xdr:rowOff>
+      <xdr:rowOff>1687680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4153,8 +4536,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1034640" y="794520"/>
-          <a:ext cx="3292920" cy="1664280"/>
+          <a:off x="1061640" y="785520"/>
+          <a:ext cx="3292560" cy="1663920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4169,15 +4552,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1719000</xdr:colOff>
+      <xdr:colOff>1746000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>175680</xdr:rowOff>
+      <xdr:rowOff>166680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5307120</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28440</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1762200</xdr:rowOff>
+      <xdr:rowOff>1752840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4190,8 +4573,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6913800" y="747000"/>
-          <a:ext cx="3588120" cy="1776960"/>
+          <a:off x="5822640" y="738000"/>
+          <a:ext cx="3587760" cy="1776600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4211,15 +4594,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>216000</xdr:colOff>
+      <xdr:colOff>243000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>118440</xdr:rowOff>
+      <xdr:rowOff>109440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>565560</xdr:colOff>
+      <xdr:colOff>592200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2140920</xdr:rowOff>
+      <xdr:rowOff>2131560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4232,8 +4615,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="216000" y="861120"/>
-          <a:ext cx="4490280" cy="2212920"/>
+          <a:off x="243000" y="852120"/>
+          <a:ext cx="3597120" cy="2212560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4256,17 +4639,17 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.71255060728745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7125506072875"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9959514170041"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.56632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4466,14 +4849,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="109.425101214575"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="108.265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25364,14 +25747,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="89.421052631579"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="88.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25901,14 +26284,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="126.287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="124.867346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26436,14 +26819,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="93"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="91.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26971,14 +27354,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="87.5748987854251"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="86.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27506,14 +27889,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="90.7165991902834"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="89.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28041,9 +28424,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.421052631579"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.9959514170041"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.7755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28245,9 +28628,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.1457489878543"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.4489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Actualización concentrado de métricas
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Métricas y monitoreo/Plan_Métricas_2016.xlsx
+++ b/Proyectos/2016/Métricas y monitoreo/Plan_Métricas_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Objetivos de Medición" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,16 +19,11 @@
     <sheet name="Índice de Satisfacción" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="142">
   <si>
     <t>Objetivos de Medición</t>
   </si>
@@ -39,7 +34,7 @@
     <t>Métricas</t>
   </si>
   <si>
-    <t>Tener una desviación miníma del - 15% en esfuerzo y costo de los servicios ofertados con el fin de asegurar la rentabilidad del negocio.</t>
+    <t>Tener una desviación miníma del – 15% y maxima del 15% en esfuerzo(proyectos generados) y una desviación menor o igual al 0% de costo de los servicios ofertados con el fin de asegurar la rentabilidad del negocio.</t>
   </si>
   <si>
     <t>Desviación de esfuerzo</t>
@@ -69,7 +64,7 @@
     <t>Índice de Satisfacción</t>
   </si>
   <si>
-    <t>Obtener un crecimiento anual del 40% representado por un total de 2,424,000</t>
+    <t>Obtener un crecimiento anual del 30% representado por un total de 3,300,000 pesos</t>
   </si>
   <si>
     <t>Crecimiento anual de ventas</t>
@@ -153,7 +148,7 @@
     <t>Mecanismo de Recolección y Almacenamiento</t>
   </si>
   <si>
-    <t>Ingresar al plan de proyecto en la sección estimación y tomar el valor total de los proyectos esperados anualmente y dividirlo entre los doce meses, almacenar dicho dato como esfuerzo planeado, adicional ir al sistema sos soft el cual tiene la cantidad de proyectos registrados y generar la sumatoria de los registros en color rojo, generar el calculo especificado previamente y almacenarlo en el concentrado de métricas en la pestaña esfuerzo</t>
+    <t>Ingresar al plan de proyecto en la sección estimación y tomar el valor total de los proyectos esperados anualmente y dividirlo entre los doce meses, almacenar dicho dato como esfuerzo planeado, adicional solicitar a administración la cantidad de servicios ejecutados durante el mes evaluado por parte del area de ventas, dicho resultado solo pertenece a la seccion de ventas, para obtener la sección de soporte se deberá ingresar a bitrix en la pestaña CRM, Activities ,presionar el botón mas y poner iniciales de persona a filtrar,  presionar el cuadro posicionado a la derecha del botón mas e ingresar nombre de persona y tareas completas (se puede filtrar por deadline), generar el calculo especificado previamente y almacenarlo en el concentrado de métricas en la pestaña esfuerzo</t>
   </si>
   <si>
     <t>Periodicidad</t>
@@ -183,42 +178,25 @@
     <t>A quien se presenta el reporte de métricas</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Guía de análisis:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
+    <t>Guía de análisis: </t>
   </si>
   <si>
     <t>El análisis se hara en base a la grafica de Desviación</t>
   </si>
   <si>
-    <t>Si la desviación es mayor o igual al 0%</t>
+    <t>Si la desviación se encuentra entre el 15% y -15%</t>
   </si>
   <si>
     <t>Se continua con el seguimiento</t>
   </si>
   <si>
-    <t>Si la desviación es menor al 0 % y mayor al -15%</t>
+    <t>Si la desviación se encuentra entre el 16% y el 30% positivo o negativo</t>
   </si>
   <si>
     <t>Se monitorea y analiza con dirección, se toman acciones para reducir la desviación</t>
   </si>
   <si>
-    <t>Si la desviación es menor al -15% </t>
+    <t>Si la es superior al 31% positivo o negativo</t>
   </si>
   <si>
     <t>Se analiza con direccion para tomar medidas inmeditas para corregir la desviacion y considerar actualizar la estimación del servicio</t>
@@ -276,6 +254,15 @@
   </si>
   <si>
     <t>Tomar el costo estimado en el plan de proyecto dividido entre doce meses como costo planeado y tomar el total gastado entre servicios y sueldos de personal registrados en el mes, dicho dato será otorgado por administración aplicar formula de desviación en porcentaje y plasmar en el concentrado de métricas en la pestaña costos.</t>
+  </si>
+  <si>
+    <t>Si la desviación es menor o igual al 0%</t>
+  </si>
+  <si>
+    <t>Si la desviación es mayor al 0% y menor al 15%</t>
+  </si>
+  <si>
+    <t>Si la desviación es mayor al 15%</t>
   </si>
   <si>
     <t>Desviacion del costo</t>
@@ -383,7 +370,7 @@
     <t>Total obtenido mensual</t>
   </si>
   <si>
-    <t>Tomando los datos del documento control de ventas sumar el total por empleado y registrarlo en la pestaña ventas del concentrado sección venta por empleado, adicional sumar el total hasta el año y comprarlo contra lo planeado anualmente.</t>
+    <t>Solicitar la información de ventas por persona y venta total del mes al area de administración y comparar con lo planeado</t>
   </si>
   <si>
     <t>Reunión de monitoreo</t>
@@ -395,39 +382,19 @@
     <t>A quien se le presenta el reporte de métricas</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Guía de análisis:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
-    <t>Que el índice de crecimiento en ventas sea mayor o igual a 40% </t>
+    <t>Que el índice de crecimiento en ventas sea mayor o igual a 30% </t>
   </si>
   <si>
     <t>Seguimiento</t>
   </si>
   <si>
-    <t>Que el índice de ventas sea menor que 10% y mayor o igual a 39%</t>
+    <t>Que el índice de ventas sea mayor que 0% y menor o igual a 29%</t>
   </si>
   <si>
     <t>Crear plan de acción para aumentar el porcentaje de cumplimiento en ventas.</t>
   </si>
   <si>
-    <t>Que el índice de ventas sea menor o igual a 9%</t>
+    <t>Que el índice de ventas sea menor o igual a  -1%</t>
   </si>
   <si>
     <t>Crear un plan de acción en base a los malos resultados obtenidos.</t>
@@ -707,7 +674,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -820,6 +787,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -913,6 +884,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1023,13 +998,12 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1052,7 +1026,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1060,7 +1033,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1156,7 +1128,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1164,7 +1135,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1260,7 +1230,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1268,7 +1237,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1344,17 +1312,16 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="72435166"/>
-        <c:axId val="13793230"/>
+        <c:axId val="10895760"/>
+        <c:axId val="50576713"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="72435166"/>
+        <c:axId val="10895760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1366,32 +1333,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="13793230"/>
+        <c:crossAx val="50576713"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13793230"/>
+        <c:axId val="50576713"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1410,32 +1359,17 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -1443,9 +1377,8 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1457,25 +1390,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="72435166"/>
+        <c:crossAx val="10895760"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -1493,7 +1408,6 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1509,13 +1423,12 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1536,7 +1449,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1544,7 +1456,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1638,7 +1549,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1646,7 +1556,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1740,7 +1649,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -1748,7 +1656,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1824,17 +1731,16 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="18027514"/>
-        <c:axId val="80308284"/>
+        <c:axId val="78061030"/>
+        <c:axId val="86752310"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="18027514"/>
+        <c:axId val="78061030"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1846,32 +1752,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="80308284"/>
+        <c:crossAx val="86752310"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80308284"/>
+        <c:axId val="86752310"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1890,32 +1778,17 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -1923,9 +1796,8 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="\$#,##0.00;[RED]\$#,##0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1937,25 +1809,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="18027514"/>
+        <c:crossAx val="78061030"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -1973,7 +1827,6 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1989,13 +1842,12 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2018,7 +1870,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2026,7 +1877,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2122,7 +1972,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2130,7 +1979,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2226,7 +2074,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2234,7 +2081,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2310,17 +2156,16 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="98391957"/>
-        <c:axId val="63067750"/>
+        <c:axId val="60688100"/>
+        <c:axId val="41526891"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="98391957"/>
+        <c:axId val="60688100"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2332,32 +2177,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="63067750"/>
+        <c:crossAx val="41526891"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63067750"/>
+        <c:axId val="41526891"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2376,32 +2203,17 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -2409,9 +2221,8 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2423,25 +2234,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="98391957"/>
+        <c:crossAx val="60688100"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -2459,7 +2252,6 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2475,13 +2267,12 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2504,7 +2295,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2512,7 +2302,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2608,7 +2397,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2616,7 +2404,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2712,7 +2499,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2720,7 +2506,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -2796,17 +2581,16 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="92254162"/>
-        <c:axId val="70893083"/>
+        <c:axId val="93637125"/>
+        <c:axId val="35290820"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92254162"/>
+        <c:axId val="93637125"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2818,32 +2602,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="70893083"/>
+        <c:crossAx val="35290820"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70893083"/>
+        <c:axId val="35290820"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2862,32 +2628,17 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -2895,9 +2646,8 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2909,25 +2659,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="92254162"/>
+        <c:crossAx val="93637125"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -2945,7 +2677,6 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2961,13 +2692,12 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2990,7 +2720,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -2998,7 +2727,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3094,7 +2822,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -3102,7 +2829,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3198,7 +2924,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -3206,7 +2931,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3282,17 +3006,16 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="65908345"/>
-        <c:axId val="86565072"/>
+        <c:axId val="51910841"/>
+        <c:axId val="83730812"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="65908345"/>
+        <c:axId val="51910841"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3304,32 +3027,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="86565072"/>
+        <c:crossAx val="83730812"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86565072"/>
+        <c:axId val="83730812"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3348,32 +3053,17 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -3381,9 +3071,8 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3395,25 +3084,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="65908345"/>
+        <c:crossAx val="51910841"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -3431,7 +3102,6 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3447,13 +3117,12 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3476,7 +3145,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -3484,7 +3152,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3580,7 +3247,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -3588,7 +3254,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3684,7 +3349,6 @@
               <a:noFill/>
             </a:ln>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
@@ -3692,7 +3356,6 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3768,17 +3431,16 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="60765664"/>
-        <c:axId val="95054219"/>
+        <c:axId val="19635523"/>
+        <c:axId val="1983556"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="60765664"/>
+        <c:axId val="19635523"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3790,32 +3452,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="95054219"/>
+        <c:crossAx val="1983556"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95054219"/>
+        <c:axId val="1983556"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3834,32 +3478,17 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000"/>
+              <a:bodyPr/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="1000">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:uFill>
-                      <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
-                      </a:solidFill>
-                    </a:uFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
                   <a:t>Axis Title</a:t>
@@ -3867,9 +3496,8 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
+          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3881,25 +3509,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="60765664"/>
+        <c:crossAx val="19635523"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -3917,7 +3527,6 @@
       </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3935,15 +3544,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>471600</xdr:colOff>
+      <xdr:colOff>633600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>72720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>354240</xdr:colOff>
+      <xdr:colOff>514080</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>95760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3951,8 +3560,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="34513920" y="9330120"/>
-        <a:ext cx="4626000" cy="2882520"/>
+        <a:off x="43534800" y="10135440"/>
+        <a:ext cx="5858280" cy="2880360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3965,15 +3574,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>405360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>111960</xdr:rowOff>
+      <xdr:rowOff>57960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3312000</xdr:colOff>
+      <xdr:colOff>3472200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2032920</xdr:rowOff>
+      <xdr:rowOff>1977120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3986,8 +3595,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="395280" y="680760"/>
-          <a:ext cx="5345280" cy="2111400"/>
+          <a:off x="596880" y="626760"/>
+          <a:ext cx="5935680" cy="2109600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4002,15 +3611,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3500640</xdr:colOff>
+      <xdr:colOff>3663000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>169200</xdr:rowOff>
+      <xdr:rowOff>115200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7479000</xdr:colOff>
+      <xdr:colOff>7639200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1988640</xdr:rowOff>
+      <xdr:rowOff>1932840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4023,8 +3632,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5929200" y="738000"/>
-          <a:ext cx="3978360" cy="2009880"/>
+          <a:off x="6723360" y="684000"/>
+          <a:ext cx="3976200" cy="2008080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4044,15 +3653,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>420840</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:colOff>582840</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>168480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>392040</xdr:colOff>
+      <xdr:colOff>551880</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4060,8 +3669,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33853320" y="9836280"/>
-        <a:ext cx="6296040" cy="3349800"/>
+        <a:off x="42715080" y="9782280"/>
+        <a:ext cx="7939440" cy="3347640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4074,15 +3683,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>405000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>299880</xdr:rowOff>
+      <xdr:rowOff>245880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2220840</xdr:colOff>
+      <xdr:colOff>2380680</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2183760</xdr:rowOff>
+      <xdr:rowOff>2127600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4095,8 +3704,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="395280" y="871200"/>
-          <a:ext cx="4254120" cy="2434320"/>
+          <a:off x="596520" y="817200"/>
+          <a:ext cx="4844520" cy="2432160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4111,15 +3720,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2243160</xdr:colOff>
+      <xdr:colOff>2405160</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>271440</xdr:rowOff>
+      <xdr:rowOff>217440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>258840</xdr:colOff>
+      <xdr:colOff>418680</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2172240</xdr:rowOff>
+      <xdr:rowOff>2116080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4132,8 +3741,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4671720" y="842760"/>
-          <a:ext cx="4254840" cy="2451240"/>
+          <a:off x="5465520" y="788760"/>
+          <a:ext cx="5875560" cy="2449080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4153,15 +3762,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>471600</xdr:colOff>
+      <xdr:colOff>633600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>6840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>354240</xdr:colOff>
+      <xdr:colOff>514080</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4169,8 +3778,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="35685360" y="9053640"/>
-        <a:ext cx="4626000" cy="2882880"/>
+        <a:off x="45010440" y="8999640"/>
+        <a:ext cx="5858280" cy="2880720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4183,15 +3792,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>405000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>56880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4091040</xdr:colOff>
+      <xdr:colOff>4250880</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2288880</xdr:rowOff>
+      <xdr:rowOff>2232720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4204,8 +3813,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="395280" y="718920"/>
-          <a:ext cx="6124320" cy="2368440"/>
+          <a:off x="596520" y="664920"/>
+          <a:ext cx="6714720" cy="2366280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4220,15 +3829,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4757760</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:colOff>4919760</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>199800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>8555040</xdr:colOff>
+      <xdr:colOff>8714880</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2266560</xdr:rowOff>
+      <xdr:rowOff>2210400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4241,8 +3850,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7186320" y="633240"/>
-          <a:ext cx="3797280" cy="2431800"/>
+          <a:off x="7980120" y="579240"/>
+          <a:ext cx="3795120" cy="2429640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4262,15 +3871,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>471600</xdr:colOff>
+      <xdr:colOff>633600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>59760</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>354240</xdr:colOff>
+      <xdr:colOff>514080</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4278,8 +3887,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33361200" y="9272880"/>
-        <a:ext cx="4626000" cy="2882520"/>
+        <a:off x="42081840" y="9218880"/>
+        <a:ext cx="5858280" cy="2880360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4292,15 +3901,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>405000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2247480</xdr:colOff>
+      <xdr:colOff>2407320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2325600</xdr:rowOff>
+      <xdr:rowOff>2269440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4313,8 +3922,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="395280" y="871200"/>
-          <a:ext cx="4280760" cy="2406600"/>
+          <a:off x="596520" y="817200"/>
+          <a:ext cx="4871160" cy="2404440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4329,15 +3938,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2274120</xdr:colOff>
+      <xdr:colOff>2436120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>90360</xdr:rowOff>
+      <xdr:rowOff>36360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6421320</xdr:colOff>
+      <xdr:colOff>6581160</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2340360</xdr:rowOff>
+      <xdr:rowOff>2284200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4350,8 +3959,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4702680" y="852120"/>
-          <a:ext cx="4147200" cy="2440440"/>
+          <a:off x="5496480" y="798120"/>
+          <a:ext cx="4145040" cy="2438280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4371,15 +3980,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>471600</xdr:colOff>
+      <xdr:colOff>633600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>59760</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>354240</xdr:colOff>
+      <xdr:colOff>514080</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>28800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4387,8 +3996,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="32980320" y="9194760"/>
-        <a:ext cx="4626000" cy="2882520"/>
+        <a:off x="41601600" y="9140760"/>
+        <a:ext cx="5858640" cy="2880360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4401,15 +4010,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1033560</xdr:colOff>
+      <xdr:colOff>1195560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2639880</xdr:colOff>
+      <xdr:colOff>2799720</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2346480</xdr:rowOff>
+      <xdr:rowOff>2290320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4422,8 +4031,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1185840" y="680760"/>
-          <a:ext cx="3882600" cy="2427480"/>
+          <a:off x="1387080" y="626760"/>
+          <a:ext cx="4473000" cy="2425320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4443,15 +4052,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>471600</xdr:colOff>
+      <xdr:colOff>633600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>61200</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>354240</xdr:colOff>
+      <xdr:colOff>514080</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>86040</xdr:rowOff>
+      <xdr:rowOff>29880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4459,8 +4068,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="33199200" y="9109080"/>
-        <a:ext cx="4626360" cy="2882520"/>
+        <a:off x="41877360" y="9055080"/>
+        <a:ext cx="5858280" cy="2880360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4473,15 +4082,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>690840</xdr:colOff>
+      <xdr:colOff>852840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:rowOff>83880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2116440</xdr:colOff>
+      <xdr:colOff>2276280</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2262240</xdr:rowOff>
+      <xdr:rowOff>2206080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4494,8 +4103,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="843120" y="709200"/>
-          <a:ext cx="3701880" cy="2314800"/>
+          <a:off x="1044360" y="655200"/>
+          <a:ext cx="4292280" cy="2312640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4515,15 +4124,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1061640</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>23760</xdr:rowOff>
+      <xdr:colOff>1223640</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>277560</xdr:colOff>
+      <xdr:colOff>437400</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1687680</xdr:rowOff>
+      <xdr:rowOff>1631520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4536,8 +4145,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1061640" y="785520"/>
-          <a:ext cx="3292560" cy="1663920"/>
+          <a:off x="1223640" y="731520"/>
+          <a:ext cx="4351320" cy="1661760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4552,15 +4161,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1746000</xdr:colOff>
+      <xdr:colOff>1908000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>166680</xdr:rowOff>
+      <xdr:rowOff>112680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>28440</xdr:colOff>
+      <xdr:colOff>188280</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1752840</xdr:rowOff>
+      <xdr:rowOff>1696680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4573,8 +4182,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5822640" y="738000"/>
-          <a:ext cx="3587760" cy="1776600"/>
+          <a:off x="7045560" y="684000"/>
+          <a:ext cx="4966200" cy="1774440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4594,15 +4203,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>243000</xdr:colOff>
+      <xdr:colOff>405000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>109440</xdr:rowOff>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>592200</xdr:colOff>
+      <xdr:colOff>752040</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2131560</xdr:rowOff>
+      <xdr:rowOff>2075400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4615,8 +4224,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="243000" y="852120"/>
-          <a:ext cx="3597120" cy="2212560"/>
+          <a:off x="405000" y="798120"/>
+          <a:ext cx="4440240" cy="2210400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4638,18 +4247,18 @@
   </sheetPr>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.56632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.56275303643725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1093117408907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4372469635628"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7692307692308"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3886639676113"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4679,7 +4288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="56.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
         <v>5</v>
@@ -4724,7 +4333,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="8" t="s">
         <v>13</v>
       </c>
@@ -4843,20 +4452,20 @@
   </sheetPr>
   <dimension ref="1:47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="108.265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="108.267206477733"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16178,7 +15787,7 @@
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="12" customFormat="false" ht="115.65" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="27" t="s">
         <v>40</v>
@@ -24416,10 +24025,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A20" s="0"/>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="0"/>
       <c r="E20" s="0"/>
       <c r="F20" s="0"/>
@@ -25442,17 +25051,17 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" s="28" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B21" s="29" t="s">
+    <row r="21" s="29" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="B21" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="29"/>
+      <c r="C21" s="30"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="32" t="s">
         <v>53</v>
       </c>
       <c r="AA22" s="0"/>
@@ -25461,7 +25070,7 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="33" t="s">
         <v>54</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -25473,7 +25082,7 @@
       <c r="AD23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="34" t="s">
         <v>56</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -25586,7 +25195,7 @@
       <c r="AC39" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="AD39" s="34" t="n">
+      <c r="AD39" s="35" t="n">
         <f aca="false">(AC39-AB39)/100</f>
         <v>-0.2</v>
       </c>
@@ -25601,7 +25210,7 @@
       <c r="AC40" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="AD40" s="34" t="n">
+      <c r="AD40" s="35" t="n">
         <f aca="false">(AC40-AB40)/100</f>
         <v>-1.81</v>
       </c>
@@ -25616,7 +25225,7 @@
       <c r="AC41" s="22" t="n">
         <v>343</v>
       </c>
-      <c r="AD41" s="34" t="n">
+      <c r="AD41" s="35" t="n">
         <f aca="false">(AC41-AB41)/100</f>
         <v>-2</v>
       </c>
@@ -25631,7 +25240,7 @@
       <c r="AC42" s="22" t="n">
         <v>331</v>
       </c>
-      <c r="AD42" s="34" t="n">
+      <c r="AD42" s="35" t="n">
         <f aca="false">(AC42-AB42)/100</f>
         <v>-0.11</v>
       </c>
@@ -25646,7 +25255,7 @@
       <c r="AC43" s="22" t="n">
         <v>434</v>
       </c>
-      <c r="AD43" s="34" t="n">
+      <c r="AD43" s="35" t="n">
         <f aca="false">(AC43-AB43)/100</f>
         <v>0.9</v>
       </c>
@@ -25661,7 +25270,7 @@
       <c r="AC44" s="22" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="34" t="n">
+      <c r="AD44" s="35" t="n">
         <f aca="false">(AC44-AB44)/100</f>
         <v>0.01</v>
       </c>
@@ -25676,7 +25285,7 @@
       <c r="AC45" s="22" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="34" t="n">
+      <c r="AD45" s="35" t="n">
         <f aca="false">(AC45-AB45)/100</f>
         <v>0</v>
       </c>
@@ -25691,7 +25300,7 @@
       <c r="AC46" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="AD46" s="34" t="n">
+      <c r="AD46" s="35" t="n">
         <f aca="false">(AC46-AB46)/100</f>
         <v>0.1</v>
       </c>
@@ -25706,7 +25315,7 @@
       <c r="AC47" s="22" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="34" t="n">
+      <c r="AD47" s="35" t="n">
         <f aca="false">(AC47-AB47)/100</f>
         <v>0.18</v>
       </c>
@@ -25741,20 +25350,20 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="88.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="88.417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25971,20 +25580,20 @@
       <c r="AD19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B21" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="31" t="s">
+      <c r="B21" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="32" t="s">
         <v>53</v>
       </c>
       <c r="AA21" s="0"/>
@@ -25993,8 +25602,8 @@
       <c r="AD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="32" t="s">
-        <v>54</v>
+      <c r="B22" s="33" t="s">
+        <v>77</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>55</v>
@@ -26005,8 +25614,8 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="33" t="s">
-        <v>56</v>
+      <c r="B23" s="34" t="s">
+        <v>78</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>57</v>
@@ -26111,20 +25720,20 @@
         <v>73</v>
       </c>
       <c r="AD38" s="22" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA39" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AB39" s="35" t="n">
+      <c r="AB39" s="36" t="n">
         <v>3287</v>
       </c>
-      <c r="AC39" s="35" t="n">
+      <c r="AC39" s="36" t="n">
         <v>4076</v>
       </c>
-      <c r="AD39" s="36" t="n">
+      <c r="AD39" s="37" t="n">
         <f aca="false">(AC39-AB39)</f>
         <v>789</v>
       </c>
@@ -26133,13 +25742,13 @@
       <c r="AA40" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AB40" s="35" t="n">
+      <c r="AB40" s="36" t="n">
         <v>5344</v>
       </c>
-      <c r="AC40" s="35" t="n">
+      <c r="AC40" s="36" t="n">
         <v>4088</v>
       </c>
-      <c r="AD40" s="36" t="n">
+      <c r="AD40" s="37" t="n">
         <f aca="false">(AC40-AB40)</f>
         <v>-1256</v>
       </c>
@@ -26148,13 +25757,13 @@
       <c r="AA41" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="AB41" s="35" t="n">
+      <c r="AB41" s="36" t="n">
         <v>3423</v>
       </c>
-      <c r="AC41" s="35" t="n">
+      <c r="AC41" s="36" t="n">
         <v>5076</v>
       </c>
-      <c r="AD41" s="36" t="n">
+      <c r="AD41" s="37" t="n">
         <f aca="false">(AC41-AB41)</f>
         <v>1653</v>
       </c>
@@ -26163,13 +25772,13 @@
       <c r="AA42" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="AB42" s="35" t="n">
+      <c r="AB42" s="36" t="n">
         <v>40000</v>
       </c>
-      <c r="AC42" s="35" t="n">
+      <c r="AC42" s="36" t="n">
         <v>37000</v>
       </c>
-      <c r="AD42" s="36" t="n">
+      <c r="AD42" s="37" t="n">
         <f aca="false">(AC42-AB42)</f>
         <v>-3000</v>
       </c>
@@ -26178,13 +25787,13 @@
       <c r="AA43" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="AB43" s="35" t="n">
+      <c r="AB43" s="36" t="n">
         <v>5467</v>
       </c>
-      <c r="AC43" s="35" t="n">
+      <c r="AC43" s="36" t="n">
         <v>4980</v>
       </c>
-      <c r="AD43" s="36" t="n">
+      <c r="AD43" s="37" t="n">
         <f aca="false">(AC43-AB43)</f>
         <v>-487</v>
       </c>
@@ -26193,13 +25802,13 @@
       <c r="AA44" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="AB44" s="35" t="n">
+      <c r="AB44" s="36" t="n">
         <v>532</v>
       </c>
-      <c r="AC44" s="35" t="n">
+      <c r="AC44" s="36" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="36" t="n">
+      <c r="AD44" s="37" t="n">
         <f aca="false">(AC44-AB44)</f>
         <v>1</v>
       </c>
@@ -26208,13 +25817,13 @@
       <c r="AA45" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="AB45" s="35" t="n">
+      <c r="AB45" s="36" t="n">
         <v>534</v>
       </c>
-      <c r="AC45" s="35" t="n">
+      <c r="AC45" s="36" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="36" t="n">
+      <c r="AD45" s="37" t="n">
         <f aca="false">(AC45-AB45)</f>
         <v>0</v>
       </c>
@@ -26223,13 +25832,13 @@
       <c r="AA46" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="AB46" s="35" t="n">
+      <c r="AB46" s="36" t="n">
         <v>900</v>
       </c>
-      <c r="AC46" s="35" t="n">
+      <c r="AC46" s="36" t="n">
         <v>1500</v>
       </c>
-      <c r="AD46" s="36" t="n">
+      <c r="AD46" s="37" t="n">
         <f aca="false">(AC46-AB46)</f>
         <v>600</v>
       </c>
@@ -26238,13 +25847,13 @@
       <c r="AA47" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="AB47" s="35" t="n">
+      <c r="AB47" s="36" t="n">
         <v>324</v>
       </c>
-      <c r="AC47" s="35" t="n">
+      <c r="AC47" s="36" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="36" t="n">
+      <c r="AD47" s="37" t="n">
         <f aca="false">(AC47-AB47)</f>
         <v>18</v>
       </c>
@@ -26278,24 +25887,24 @@
   </sheetPr>
   <dimension ref="B1:AD47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="124.867346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="124.866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="14" t="str">
@@ -26312,7 +25921,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
@@ -26324,7 +25933,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="AA3" s="0"/>
       <c r="AB3" s="0"/>
@@ -26373,10 +25982,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B8" s="27" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="AA8" s="0"/>
       <c r="AB8" s="0"/>
@@ -26385,7 +25994,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B9" s="27" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C9" s="18"/>
       <c r="AA9" s="0"/>
@@ -26395,7 +26004,7 @@
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B10" s="27" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C10" s="18"/>
       <c r="AA10" s="0"/>
@@ -26415,7 +26024,7 @@
     </row>
     <row r="12" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B12" s="27" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C12" s="27"/>
       <c r="AA12" s="0"/>
@@ -26474,7 +26083,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AA17" s="0"/>
       <c r="AB17" s="0"/>
@@ -26506,21 +26115,21 @@
       <c r="AD19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B21" s="38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>86</v>
+      <c r="B21" s="39" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>89</v>
       </c>
       <c r="AA21" s="0"/>
       <c r="AB21" s="0"/>
@@ -26528,11 +26137,11 @@
       <c r="AD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="40" t="s">
-        <v>87</v>
+      <c r="B22" s="41" t="s">
+        <v>90</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
@@ -26540,11 +26149,11 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="41" t="s">
-        <v>89</v>
+      <c r="B23" s="42" t="s">
+        <v>92</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AA23" s="0"/>
       <c r="AB23" s="0"/>
@@ -26659,7 +26268,7 @@
       <c r="AC39" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="AD39" s="34" t="n">
+      <c r="AD39" s="35" t="n">
         <f aca="false">(AC39-AB39)/100</f>
         <v>-0.2</v>
       </c>
@@ -26674,7 +26283,7 @@
       <c r="AC40" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="AD40" s="34" t="n">
+      <c r="AD40" s="35" t="n">
         <f aca="false">(AC40-AB40)/100</f>
         <v>-1.81</v>
       </c>
@@ -26689,7 +26298,7 @@
       <c r="AC41" s="22" t="n">
         <v>343</v>
       </c>
-      <c r="AD41" s="34" t="n">
+      <c r="AD41" s="35" t="n">
         <f aca="false">(AC41-AB41)/100</f>
         <v>-2</v>
       </c>
@@ -26704,7 +26313,7 @@
       <c r="AC42" s="22" t="n">
         <v>331</v>
       </c>
-      <c r="AD42" s="34" t="n">
+      <c r="AD42" s="35" t="n">
         <f aca="false">(AC42-AB42)/100</f>
         <v>-0.11</v>
       </c>
@@ -26719,7 +26328,7 @@
       <c r="AC43" s="22" t="n">
         <v>434</v>
       </c>
-      <c r="AD43" s="34" t="n">
+      <c r="AD43" s="35" t="n">
         <f aca="false">(AC43-AB43)/100</f>
         <v>0.9</v>
       </c>
@@ -26734,7 +26343,7 @@
       <c r="AC44" s="22" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="34" t="n">
+      <c r="AD44" s="35" t="n">
         <f aca="false">(AC44-AB44)/100</f>
         <v>0.01</v>
       </c>
@@ -26749,7 +26358,7 @@
       <c r="AC45" s="22" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="34" t="n">
+      <c r="AD45" s="35" t="n">
         <f aca="false">(AC45-AB45)/100</f>
         <v>0</v>
       </c>
@@ -26764,7 +26373,7 @@
       <c r="AC46" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="AD46" s="34" t="n">
+      <c r="AD46" s="35" t="n">
         <f aca="false">(AC46-AB46)/100</f>
         <v>0.1</v>
       </c>
@@ -26779,7 +26388,7 @@
       <c r="AC47" s="22" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="34" t="n">
+      <c r="AD47" s="35" t="n">
         <f aca="false">(AC47-AB47)/100</f>
         <v>0.18</v>
       </c>
@@ -26819,18 +26428,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="91.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="91.9311740890688"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="14" t="str">
@@ -26847,7 +26456,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
@@ -26859,7 +26468,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="AA3" s="0"/>
       <c r="AB3" s="0"/>
@@ -26908,10 +26517,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B8" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>93</v>
+        <v>82</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>96</v>
       </c>
       <c r="AA8" s="0"/>
       <c r="AB8" s="0"/>
@@ -26920,9 +26529,9 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B9" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="42"/>
+        <v>84</v>
+      </c>
+      <c r="C9" s="43"/>
       <c r="AA9" s="0"/>
       <c r="AB9" s="0"/>
       <c r="AC9" s="0"/>
@@ -26930,9 +26539,9 @@
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B10" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="42"/>
+        <v>85</v>
+      </c>
+      <c r="C10" s="43"/>
       <c r="AA10" s="0"/>
       <c r="AB10" s="0"/>
       <c r="AC10" s="0"/>
@@ -26950,7 +26559,7 @@
     </row>
     <row r="12" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B12" s="27" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C12" s="27"/>
       <c r="AA12" s="0"/>
@@ -27009,7 +26618,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="AA17" s="0"/>
       <c r="AB17" s="0"/>
@@ -27041,21 +26650,21 @@
       <c r="AD19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B21" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>86</v>
+      <c r="B21" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>89</v>
       </c>
       <c r="AA21" s="0"/>
       <c r="AB21" s="0"/>
@@ -27063,11 +26672,11 @@
       <c r="AD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="40" t="s">
-        <v>87</v>
+      <c r="B22" s="41" t="s">
+        <v>90</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
@@ -27075,11 +26684,11 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="41" t="s">
-        <v>89</v>
+      <c r="B23" s="42" t="s">
+        <v>92</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AA23" s="0"/>
       <c r="AB23" s="0"/>
@@ -27194,7 +26803,7 @@
       <c r="AC39" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="AD39" s="34" t="n">
+      <c r="AD39" s="35" t="n">
         <f aca="false">(AC39-AB39)/100</f>
         <v>-0.2</v>
       </c>
@@ -27209,7 +26818,7 @@
       <c r="AC40" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="AD40" s="34" t="n">
+      <c r="AD40" s="35" t="n">
         <f aca="false">(AC40-AB40)/100</f>
         <v>-1.81</v>
       </c>
@@ -27224,7 +26833,7 @@
       <c r="AC41" s="22" t="n">
         <v>343</v>
       </c>
-      <c r="AD41" s="34" t="n">
+      <c r="AD41" s="35" t="n">
         <f aca="false">(AC41-AB41)/100</f>
         <v>-2</v>
       </c>
@@ -27239,7 +26848,7 @@
       <c r="AC42" s="22" t="n">
         <v>331</v>
       </c>
-      <c r="AD42" s="34" t="n">
+      <c r="AD42" s="35" t="n">
         <f aca="false">(AC42-AB42)/100</f>
         <v>-0.11</v>
       </c>
@@ -27254,7 +26863,7 @@
       <c r="AC43" s="22" t="n">
         <v>434</v>
       </c>
-      <c r="AD43" s="34" t="n">
+      <c r="AD43" s="35" t="n">
         <f aca="false">(AC43-AB43)/100</f>
         <v>0.9</v>
       </c>
@@ -27269,7 +26878,7 @@
       <c r="AC44" s="22" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="34" t="n">
+      <c r="AD44" s="35" t="n">
         <f aca="false">(AC44-AB44)/100</f>
         <v>0.01</v>
       </c>
@@ -27284,7 +26893,7 @@
       <c r="AC45" s="22" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="34" t="n">
+      <c r="AD45" s="35" t="n">
         <f aca="false">(AC45-AB45)/100</f>
         <v>0</v>
       </c>
@@ -27299,7 +26908,7 @@
       <c r="AC46" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="AD46" s="34" t="n">
+      <c r="AD46" s="35" t="n">
         <f aca="false">(AC46-AB46)/100</f>
         <v>0.1</v>
       </c>
@@ -27314,7 +26923,7 @@
       <c r="AC47" s="22" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="34" t="n">
+      <c r="AD47" s="35" t="n">
         <f aca="false">(AC47-AB47)/100</f>
         <v>0.18</v>
       </c>
@@ -27354,18 +26963,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="86.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="86.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="14" t="str">
@@ -27382,7 +26991,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
@@ -27394,7 +27003,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="AA3" s="0"/>
       <c r="AB3" s="0"/>
@@ -27443,10 +27052,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B8" s="27" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AA8" s="0"/>
       <c r="AB8" s="0"/>
@@ -27455,7 +27064,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B9" s="27" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C9" s="18"/>
       <c r="AA9" s="0"/>
@@ -27465,7 +27074,7 @@
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B10" s="27" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C10" s="18"/>
       <c r="AA10" s="0"/>
@@ -27485,7 +27094,7 @@
     </row>
     <row r="12" customFormat="false" ht="46.9" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B12" s="27" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C12" s="27"/>
       <c r="AA12" s="0"/>
@@ -27544,7 +27153,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="AA17" s="0"/>
       <c r="AB17" s="0"/>
@@ -27576,21 +27185,21 @@
       <c r="AD19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B21" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>86</v>
+      <c r="B21" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>89</v>
       </c>
       <c r="AA21" s="0"/>
       <c r="AB21" s="0"/>
@@ -27598,11 +27207,11 @@
       <c r="AD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="40" t="s">
-        <v>87</v>
+      <c r="B22" s="41" t="s">
+        <v>90</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
@@ -27610,11 +27219,11 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="41" t="s">
-        <v>89</v>
+      <c r="B23" s="42" t="s">
+        <v>92</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AA23" s="0"/>
       <c r="AB23" s="0"/>
@@ -27729,7 +27338,7 @@
       <c r="AC39" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="AD39" s="34" t="n">
+      <c r="AD39" s="35" t="n">
         <f aca="false">(AC39-AB39)/100</f>
         <v>-0.2</v>
       </c>
@@ -27744,7 +27353,7 @@
       <c r="AC40" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="AD40" s="34" t="n">
+      <c r="AD40" s="35" t="n">
         <f aca="false">(AC40-AB40)/100</f>
         <v>-1.81</v>
       </c>
@@ -27759,7 +27368,7 @@
       <c r="AC41" s="22" t="n">
         <v>343</v>
       </c>
-      <c r="AD41" s="34" t="n">
+      <c r="AD41" s="35" t="n">
         <f aca="false">(AC41-AB41)/100</f>
         <v>-2</v>
       </c>
@@ -27774,7 +27383,7 @@
       <c r="AC42" s="22" t="n">
         <v>331</v>
       </c>
-      <c r="AD42" s="34" t="n">
+      <c r="AD42" s="35" t="n">
         <f aca="false">(AC42-AB42)/100</f>
         <v>-0.11</v>
       </c>
@@ -27789,7 +27398,7 @@
       <c r="AC43" s="22" t="n">
         <v>434</v>
       </c>
-      <c r="AD43" s="34" t="n">
+      <c r="AD43" s="35" t="n">
         <f aca="false">(AC43-AB43)/100</f>
         <v>0.9</v>
       </c>
@@ -27804,7 +27413,7 @@
       <c r="AC44" s="22" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="34" t="n">
+      <c r="AD44" s="35" t="n">
         <f aca="false">(AC44-AB44)/100</f>
         <v>0.01</v>
       </c>
@@ -27819,7 +27428,7 @@
       <c r="AC45" s="22" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="34" t="n">
+      <c r="AD45" s="35" t="n">
         <f aca="false">(AC45-AB45)/100</f>
         <v>0</v>
       </c>
@@ -27834,7 +27443,7 @@
       <c r="AC46" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="AD46" s="34" t="n">
+      <c r="AD46" s="35" t="n">
         <f aca="false">(AC46-AB46)/100</f>
         <v>0.1</v>
       </c>
@@ -27849,7 +27458,7 @@
       <c r="AC47" s="22" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="34" t="n">
+      <c r="AD47" s="35" t="n">
         <f aca="false">(AC47-AB47)/100</f>
         <v>0.18</v>
       </c>
@@ -27889,18 +27498,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="89.6326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="89.6315789473684"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="14" t="str">
@@ -27917,7 +27526,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
@@ -27929,7 +27538,7 @@
         <v>69</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="AA3" s="0"/>
       <c r="AB3" s="0"/>
@@ -27978,10 +27587,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B8" s="27" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="AA8" s="0"/>
       <c r="AB8" s="0"/>
@@ -27990,7 +27599,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B9" s="27" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C9" s="18"/>
       <c r="AA9" s="0"/>
@@ -28000,7 +27609,7 @@
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B10" s="27" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C10" s="18"/>
       <c r="AA10" s="0"/>
@@ -28020,7 +27629,7 @@
     </row>
     <row r="12" customFormat="false" ht="45.6" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B12" s="27" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C12" s="27"/>
       <c r="AA12" s="0"/>
@@ -28079,7 +27688,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="AA17" s="0"/>
       <c r="AB17" s="0"/>
@@ -28111,21 +27720,21 @@
       <c r="AD19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B21" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>86</v>
+      <c r="B21" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>89</v>
       </c>
       <c r="AA21" s="0"/>
       <c r="AB21" s="0"/>
@@ -28133,11 +27742,11 @@
       <c r="AD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="40" t="s">
-        <v>87</v>
+      <c r="B22" s="41" t="s">
+        <v>90</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
@@ -28145,11 +27754,11 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="41" t="s">
-        <v>89</v>
+      <c r="B23" s="42" t="s">
+        <v>92</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AA23" s="0"/>
       <c r="AB23" s="0"/>
@@ -28264,7 +27873,7 @@
       <c r="AC39" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="AD39" s="34" t="n">
+      <c r="AD39" s="35" t="n">
         <f aca="false">(AC39-AB39)/100</f>
         <v>-0.2</v>
       </c>
@@ -28279,7 +27888,7 @@
       <c r="AC40" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="AD40" s="34" t="n">
+      <c r="AD40" s="35" t="n">
         <f aca="false">(AC40-AB40)/100</f>
         <v>-1.81</v>
       </c>
@@ -28294,7 +27903,7 @@
       <c r="AC41" s="22" t="n">
         <v>343</v>
       </c>
-      <c r="AD41" s="34" t="n">
+      <c r="AD41" s="35" t="n">
         <f aca="false">(AC41-AB41)/100</f>
         <v>-2</v>
       </c>
@@ -28309,7 +27918,7 @@
       <c r="AC42" s="22" t="n">
         <v>331</v>
       </c>
-      <c r="AD42" s="34" t="n">
+      <c r="AD42" s="35" t="n">
         <f aca="false">(AC42-AB42)/100</f>
         <v>-0.11</v>
       </c>
@@ -28324,7 +27933,7 @@
       <c r="AC43" s="22" t="n">
         <v>434</v>
       </c>
-      <c r="AD43" s="34" t="n">
+      <c r="AD43" s="35" t="n">
         <f aca="false">(AC43-AB43)/100</f>
         <v>0.9</v>
       </c>
@@ -28339,7 +27948,7 @@
       <c r="AC44" s="22" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="34" t="n">
+      <c r="AD44" s="35" t="n">
         <f aca="false">(AC44-AB44)/100</f>
         <v>0.01</v>
       </c>
@@ -28354,7 +27963,7 @@
       <c r="AC45" s="22" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="34" t="n">
+      <c r="AD45" s="35" t="n">
         <f aca="false">(AC45-AB45)/100</f>
         <v>0</v>
       </c>
@@ -28369,7 +27978,7 @@
       <c r="AC46" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="AD46" s="34" t="n">
+      <c r="AD46" s="35" t="n">
         <f aca="false">(AC46-AB46)/100</f>
         <v>0.1</v>
       </c>
@@ -28384,7 +27993,7 @@
       <c r="AC47" s="22" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="34" t="n">
+      <c r="AD47" s="35" t="n">
         <f aca="false">(AC47-AB47)/100</f>
         <v>0.18</v>
       </c>
@@ -28418,102 +28027,102 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.7755102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.1887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.1902834008097"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.3886639676113"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="46" t="s">
-        <v>104</v>
+      <c r="B2" s="47" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>105</v>
+      <c r="B3" s="47" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="48"/>
     </row>
     <row r="5" customFormat="false" ht="141" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="47"/>
+      <c r="B6" s="48"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="47" t="s">
-        <v>106</v>
+      <c r="B7" s="48" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="50" t="s">
-        <v>108</v>
+      <c r="A8" s="50" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="50"/>
+      <c r="A9" s="50" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="51"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="B10" s="50"/>
+        <v>113</v>
+      </c>
+      <c r="B10" s="51"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="47"/>
+      <c r="B11" s="48"/>
     </row>
     <row r="12" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="51" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12" s="51"/>
+      <c r="A12" s="52" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="52"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="48" t="s">
         <v>42</v>
       </c>
     </row>
@@ -28526,16 +28135,16 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="47"/>
+      <c r="B15" s="48"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="48" t="s">
         <v>46</v>
       </c>
     </row>
@@ -28544,15 +28153,15 @@
         <v>43</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>114</v>
+      <c r="A18" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="48" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28564,33 +28173,33 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="B20" s="47"/>
+      <c r="A20" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="53"/>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="52" t="s">
-        <v>116</v>
+      <c r="A21" s="54" t="s">
+        <v>118</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="53" t="s">
-        <v>118</v>
+      <c r="A22" s="55" t="s">
+        <v>120</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="54" t="s">
-        <v>120</v>
+      <c r="A23" s="56" t="s">
+        <v>122</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -28628,76 +28237,76 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.4489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="55" t="str">
+      <c r="B1" s="57" t="str">
         <f aca="false">'Objetivos de Medición'!C9</f>
         <v>Índice de Satisfacción</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="46" t="s">
-        <v>122</v>
+      <c r="B2" s="47" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="46" t="s">
-        <v>123</v>
+      <c r="B3" s="47" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="57"/>
+      <c r="B4" s="59"/>
     </row>
     <row r="5" customFormat="false" ht="184.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
+      <c r="A5" s="60"/>
+      <c r="B5" s="60"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="47"/>
+      <c r="B6" s="48"/>
       <c r="Q6" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="47" t="s">
-        <v>106</v>
+      <c r="B7" s="48" t="s">
+        <v>109</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">AVERAGE(R7:U7)</f>
@@ -28718,13 +28327,13 @@
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="Q8" s="0" t="n">
         <f aca="false">AVERAGE(R8:U8)</f>
@@ -28744,22 +28353,22 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="47"/>
+      <c r="B9" s="48"/>
     </row>
     <row r="10" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="B10" s="51"/>
+      <c r="A10" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="52"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="48" t="s">
         <v>42</v>
       </c>
     </row>
@@ -28772,16 +28381,16 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="47"/>
+      <c r="B13" s="48"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="48" t="s">
         <v>46</v>
       </c>
     </row>
@@ -28790,15 +28399,15 @@
         <v>43</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="B16" s="47" t="s">
-        <v>114</v>
+      <c r="A16" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="48" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28810,39 +28419,39 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="47"/>
+      <c r="A18" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="53"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="B19" s="59"/>
+      <c r="A19" s="61" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="61"/>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="52" t="s">
-        <v>135</v>
+      <c r="A20" s="54" t="s">
+        <v>137</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="53" t="s">
-        <v>136</v>
+      <c r="A21" s="55" t="s">
+        <v>138</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="54" t="s">
-        <v>138</v>
+      <c r="A22" s="56" t="s">
+        <v>140</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>